<commit_message>
Dispatcher update. Process workflow finished and tested. Unused workflows must be deleted later
</commit_message>
<xml_diff>
--- a/Documentation/TaxSolver Instance List (1).xlsx
+++ b/Documentation/TaxSolver Instance List (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/Returns Taxpayer documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93585AC8-F66B-41A8-98BB-488D711AAF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{93585AC8-F66B-41A8-98BB-488D711AAF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{927B665E-76E7-4FC5-B91B-4F8ABE8D171E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44AAB872-1E4E-4FF4-9C89-3E765CB0CED9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="480">
   <si>
     <t>TaxSolver ID</t>
   </si>
@@ -1470,6 +1470,12 @@
   </si>
   <si>
     <t>Younique, LLC</t>
+  </si>
+  <si>
+    <t>TFR Legal Entity</t>
+  </si>
+  <si>
+    <t>LLRSTS</t>
   </si>
 </sst>
 </file>
@@ -1793,6 +1799,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2090,2721 +2100,3457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B5D9E0-5F12-4839-AFE3-082EC7C5A69A}">
-  <dimension ref="A1:C246"/>
+  <dimension ref="A1:D246"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B183" sqref="B183:B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="31.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="D1" s="43" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2015</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3">
+        <v>2015</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D34" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D36" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D40" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D41" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D43" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B46" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D46" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D48" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D49" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D51" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D52" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D53" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D54" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D55" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D56" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D57" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D59" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D60" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D61" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D62" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D63" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D64" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D65" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D66" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D67" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D68" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D69" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C70" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D71" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D72" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D73" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D74" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D75" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="C76" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D76" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D77" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B78" s="24" t="s">
+      <c r="B78" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D78" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B79" s="24" t="s">
+      <c r="B79" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D79" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D80" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D81" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D82" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D83" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D84" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C85" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D85" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D86" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D87" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D88" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="C89" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>178</v>
       </c>
       <c r="B90" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D90" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D91" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C92" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D92" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C93" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D93" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="D94" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="C95" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D95" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C96" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D96" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D97" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B98" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C98" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D98" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="C99" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D99" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C100" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D100" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="D101" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D102" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C103" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>206</v>
       </c>
       <c r="B104" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D104" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="B105" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="D105" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="B106" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="D106" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C107" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C107" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D107" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C108" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C108" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>216</v>
       </c>
       <c r="B109" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C109" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C109" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>218</v>
       </c>
       <c r="B110" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C110" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D110" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C111" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D111" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C112" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C112" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D112" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C113" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D113" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="B114" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="C114" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D114" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="B115" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C115" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="C115" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D115" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B116" s="27" t="s">
+      <c r="B116" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="C116" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="C116" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D116" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C117" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C117" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D117" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C118" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C118" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D118" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C119" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C119" s="4" t="s">
+      <c r="D119" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="B120" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C120" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D120" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="B121" s="8" t="s">
+      <c r="B121" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C121" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D121" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C122" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C122" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D122" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="B123" s="8" t="s">
+      <c r="B123" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C123" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="C123" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D123" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B124" s="9" t="s">
+      <c r="B124" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C124" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C124" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D124" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C125" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C125" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D125" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="B126" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C126" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="C126" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D126" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B127" s="9" t="s">
+      <c r="B127" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C127" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C127" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D127" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="B128" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C128" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C128" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D128" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="B129" s="9" t="s">
+      <c r="B129" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="C129" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="C129" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D129" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B130" s="24" t="s">
+      <c r="B130" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C130" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C130" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D130" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B131" s="24" t="s">
+      <c r="B131" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C131" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C131" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D131" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B132" s="24" t="s">
+      <c r="B132" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C132" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C132" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D132" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="C133" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D133" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C134" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C134" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D134" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="B135" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="C135" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="C135" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D135" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="B136" s="30" t="s">
+      <c r="B136" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C136" s="30" t="s">
         <v>267</v>
       </c>
-      <c r="C136" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>268</v>
       </c>
       <c r="B137" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C137" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C137" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D137" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C138" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="C138" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D138" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="B139" s="8" t="s">
+      <c r="B139" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="C139" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="C139" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>274</v>
       </c>
       <c r="B140" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C140" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="C140" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D140" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="B141" s="8" t="s">
+      <c r="B141" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C141" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="C141" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D141" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="B142" s="8" t="s">
+      <c r="B142" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="C142" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="C142" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>280</v>
       </c>
       <c r="B143" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C143" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="C143" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="10" t="s">
         <v>282</v>
       </c>
       <c r="B144" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C144" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="C144" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D144" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C145" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="C145" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D145" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="B146" s="8" t="s">
+      <c r="B146" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="C146" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="C146" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D146" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C147" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C147" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D147" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C148" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="C148" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D148" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>292</v>
       </c>
       <c r="B149" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="C149" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C149" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="B150" s="8" t="s">
+      <c r="B150" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C150" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C150" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D150" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C151" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C151" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>297</v>
       </c>
       <c r="B152" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C152" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C152" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D152" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="B153" s="8" t="s">
+      <c r="B153" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="C153" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="C153" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D153" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C154" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C154" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D154" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="32" t="s">
         <v>303</v>
       </c>
-      <c r="B155" s="33" t="s">
+      <c r="B155" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="C155" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="C155" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D155" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="B156" s="8" t="s">
+      <c r="B156" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="C156" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="C156" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>307</v>
       </c>
       <c r="B157" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C157" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="C157" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D157" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="B158" s="8" t="s">
+      <c r="B158" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C158" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="C158" s="4" t="s">
+      <c r="D158" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B159" s="19" t="s">
         <v>311</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B160" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C160" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C160" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D160" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="B161" s="8" t="s">
+      <c r="B161" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="C161" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="C161" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D161" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="B162" s="8" t="s">
+      <c r="B162" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="C162" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="C162" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D162" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="B163" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C163" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="C163" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D163" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>320</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="C164" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C164" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="B165" s="24" t="s">
+      <c r="B165" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C165" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="C165" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D165" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B166" s="18" t="s">
+      <c r="B166" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C166" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="C166" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D166" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="B167" s="34" t="s">
+      <c r="B167" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C167" s="34" t="s">
         <v>326</v>
       </c>
-      <c r="C167" s="4" t="s">
+      <c r="D167" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B168" s="18" t="s">
+      <c r="B168" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C168" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="C168" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
         <v>329</v>
       </c>
       <c r="B169" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C169" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="C169" s="4" t="s">
+      <c r="D169" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B170" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C170" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="D170" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="B171" s="34" t="s">
+      <c r="B171" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="C171" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="C171" s="4" t="s">
+      <c r="D171" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="B172" s="9" t="s">
+      <c r="B172" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C172" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="C172" s="4" t="s">
+      <c r="D172" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="B173" s="6" t="s">
+      <c r="B173" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C173" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C173" s="4" t="s">
+      <c r="D173" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B174" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="C174" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C174" s="4" t="s">
+      <c r="D174" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="B175" s="6" t="s">
+      <c r="B175" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="C175" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C175" s="4" t="s">
+      <c r="D175" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>343</v>
       </c>
       <c r="B176" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="C176" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="D176" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="C177" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="C177" s="4" t="s">
+      <c r="D177" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C178" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="C178" s="4" t="s">
+      <c r="D178" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B179" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="C179" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="C179" s="4" t="s">
+      <c r="D179" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="B180" s="34" t="s">
+      <c r="B180" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="C180" s="34" t="s">
         <v>352</v>
       </c>
-      <c r="C180" s="4" t="s">
+      <c r="D180" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B181" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C181" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="C181" s="4" t="s">
+      <c r="D181" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B182" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="C182" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C182" s="4" t="s">
+      <c r="D182" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="B183" s="6" t="s">
+      <c r="B183" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="C183" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="C183" s="4" t="s">
+      <c r="D183" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="C184" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C184" s="4" t="s">
+      <c r="D184" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B185" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C185" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C185" s="4" t="s">
+      <c r="D185" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="B186" s="34" t="s">
+      <c r="B186" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C186" s="34" t="s">
         <v>364</v>
       </c>
-      <c r="C186" s="4" t="s">
+      <c r="D186" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="36" t="s">
         <v>365</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B187" s="36" t="s">
+        <v>365</v>
+      </c>
+      <c r="C187" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="C187" s="4" t="s">
+      <c r="D187" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B188" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="C188" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="C188" s="4" t="s">
+      <c r="D188" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="B189" s="6" t="s">
+      <c r="B189" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="C189" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="C189" s="4" t="s">
+      <c r="D189" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="18" t="s">
         <v>371</v>
       </c>
       <c r="B190" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="C190" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="C190" s="4" t="s">
+      <c r="D190" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B191" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="C191" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="C191" s="4" t="s">
+      <c r="D191" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>375</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="C192" s="4" t="s">
+      <c r="C192" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D192" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B193" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C193" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="C193" s="4" t="s">
+      <c r="D193" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B194" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="C194" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C194" s="4" t="s">
+      <c r="D194" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B195" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="C195" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="C195" s="4" t="s">
+      <c r="D195" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B196" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="C196" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="C196" s="4" t="s">
+      <c r="D196" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="B197" s="6" t="s">
+      <c r="B197" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="C197" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="C197" s="4" t="s">
+      <c r="D197" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="B198" s="4" t="s">
+      <c r="B198" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="C198" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="C198" s="4" t="s">
+      <c r="D198" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B199" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="C199" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="C199" s="4" t="s">
+      <c r="D199" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="35" t="s">
         <v>390</v>
       </c>
-      <c r="B200" s="9" t="s">
+      <c r="B200" s="35" t="s">
+        <v>390</v>
+      </c>
+      <c r="C200" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="C200" s="4" t="s">
+      <c r="D200" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="22" t="s">
         <v>392</v>
       </c>
       <c r="B201" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="C201" s="22" t="s">
         <v>393</v>
       </c>
-      <c r="C201" s="4" t="s">
+      <c r="D201" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="B202" s="6" t="s">
+      <c r="B202" s="17" t="s">
+        <v>394</v>
+      </c>
+      <c r="C202" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="C202" s="4" t="s">
+      <c r="D202" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="35" t="s">
         <v>396</v>
       </c>
-      <c r="B203" s="9" t="s">
+      <c r="B203" s="35" t="s">
+        <v>396</v>
+      </c>
+      <c r="C203" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="C203" s="4" t="s">
+      <c r="D203" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="18" t="s">
         <v>398</v>
       </c>
-      <c r="B204" s="9" t="s">
+      <c r="B204" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="C204" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="C204" s="4" t="s">
+      <c r="D204" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="18" t="s">
         <v>400</v>
       </c>
-      <c r="B205" s="9" t="s">
+      <c r="B205" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="C205" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="C205" s="4" t="s">
+      <c r="D205" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="9" t="s">
         <v>402</v>
       </c>
       <c r="B206" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="C206" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="C206" s="4" t="s">
+      <c r="D206" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="B207" s="9" t="s">
+      <c r="B207" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="C207" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="C207" s="4" t="s">
+      <c r="D207" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>406</v>
       </c>
       <c r="B208" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="C208" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C208" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="B209" s="6" t="s">
+      <c r="B209" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="C209" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="C209" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D209" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="B210" s="8" t="s">
+      <c r="B210" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="C210" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="C210" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D210" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="B211" s="8" t="s">
+      <c r="B211" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="C211" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="C211" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D211" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="B212" s="8" t="s">
+      <c r="B212" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="C212" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="C212" s="4" t="s">
+      <c r="D212" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="6" t="s">
         <v>415</v>
       </c>
       <c r="B213" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="C213" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="C213" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D213" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
         <v>417</v>
       </c>
       <c r="B214" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="C214" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C214" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="B215" s="8" t="s">
+      <c r="B215" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C215" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="C215" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D215" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="B216" s="4" t="s">
+      <c r="B216" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C216" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="C216" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D216" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
         <v>422</v>
       </c>
       <c r="B217" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C217" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="C217" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D217" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="B218" s="9" t="s">
+      <c r="B218" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="C218" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C218" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D218" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="B219" s="32" t="s">
+      <c r="B219" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C219" s="32" t="s">
         <v>427</v>
       </c>
-      <c r="C219" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D219" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="B220" s="9" t="s">
+      <c r="B220" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C220" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="C220" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D220" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="B221" s="7" t="s">
+      <c r="B221" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="C221" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C221" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="9" t="s">
         <v>431</v>
       </c>
       <c r="B222" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="C222" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C222" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D222" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="B223" s="7" t="s">
+      <c r="B223" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="C223" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="C223" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D223" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="B224" s="9" t="s">
+      <c r="B224" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="C224" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="C224" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D224" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225" s="11" t="s">
         <v>437</v>
       </c>
-      <c r="B225" s="8" t="s">
+      <c r="B225" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="C225" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="C225" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D225" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="B226" s="9" t="s">
+      <c r="B226" s="14" t="s">
+        <v>439</v>
+      </c>
+      <c r="C226" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="C226" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D226" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="6" t="s">
         <v>441</v>
       </c>
       <c r="B227" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="C227" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="C227" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D227" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="B228" s="7" t="s">
+      <c r="B228" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="C228" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="C228" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D228" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="6" t="s">
         <v>445</v>
       </c>
       <c r="B229" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C229" s="6" t="s">
         <v>446</v>
       </c>
-      <c r="C229" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D229" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="B230" s="8" t="s">
+      <c r="B230" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="C230" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="C230" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D230" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="B231" s="6" t="s">
+      <c r="B231" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="C231" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C231" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="B232" s="9" t="s">
+      <c r="B232" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="C232" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="C232" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D232" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="B233" s="9" t="s">
+      <c r="B233" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C233" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="C233" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D233" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="B234" s="9" t="s">
+      <c r="B234" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C234" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="C234" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D234" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A235" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="B235" s="7" t="s">
+      <c r="B235" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="C235" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="C235" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D235" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="B236" s="7" t="s">
+      <c r="B236" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="C236" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="C236" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D236" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="B237" s="8" t="s">
+      <c r="B237" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="C237" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="C237" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D237" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238" s="9" t="s">
         <v>462</v>
       </c>
       <c r="B238" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="C238" s="9" t="s">
         <v>463</v>
       </c>
-      <c r="C238" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D238" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239" s="37" t="s">
         <v>464</v>
       </c>
       <c r="B239" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="C239" s="37" t="s">
         <v>465</v>
       </c>
-      <c r="C239" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D239" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="9" t="s">
         <v>466</v>
       </c>
       <c r="B240" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C240" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="C240" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D240" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241" s="38" t="s">
         <v>468</v>
       </c>
       <c r="B241" s="38" t="s">
+        <v>468</v>
+      </c>
+      <c r="C241" s="38" t="s">
         <v>469</v>
       </c>
-      <c r="C241" s="44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D241" s="44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A242" s="38" t="s">
         <v>470</v>
       </c>
       <c r="B242" s="38" t="s">
+        <v>470</v>
+      </c>
+      <c r="C242" s="38" t="s">
         <v>471</v>
       </c>
-      <c r="C242" s="44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D242" s="44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A243" s="38" t="s">
         <v>472</v>
       </c>
       <c r="B243" s="38" t="s">
+        <v>472</v>
+      </c>
+      <c r="C243" s="38" t="s">
         <v>473</v>
       </c>
-      <c r="C243" s="44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D243" s="44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="39" t="s">
         <v>474</v>
       </c>
-      <c r="B244" s="40" t="s">
+      <c r="B244" s="39" t="s">
+        <v>474</v>
+      </c>
+      <c r="C244" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="C244" s="44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D244" s="44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A245" s="41" t="s">
         <v>476</v>
       </c>
-      <c r="B245" s="42" t="s">
+      <c r="B245" s="41" t="s">
+        <v>476</v>
+      </c>
+      <c r="C245" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="C245" s="44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D245" s="44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="40"/>
       <c r="B246" s="40"/>
-      <c r="C246" s="44"/>
+      <c r="C246" s="40"/>
+      <c r="D246" s="44"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B226">
+  <conditionalFormatting sqref="C226">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Few changes in dispatcher
</commit_message>
<xml_diff>
--- a/Documentation/TaxSolver Instance List (1).xlsx
+++ b/Documentation/TaxSolver Instance List (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{93585AC8-F66B-41A8-98BB-488D711AAF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{927B665E-76E7-4FC5-B91B-4F8ABE8D171E}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{93585AC8-F66B-41A8-98BB-488D711AAF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F54B4379-5048-47BC-9778-16B9B3D1EECF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44AAB872-1E4E-4FF4-9C89-3E765CB0CED9}"/>
   </bookViews>
@@ -1557,7 +1557,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1585,6 +1585,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1640,7 +1646,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1769,6 +1775,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -2102,14 +2163,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B5D9E0-5F12-4839-AFE3-082EC7C5A69A}">
   <dimension ref="A1:D246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183:B245"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="31.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2117,7 +2179,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="45" t="s">
         <v>478</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -2131,7 +2193,7 @@
       <c r="A2" s="3">
         <v>2015</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="46">
         <v>2015</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2145,7 +2207,7 @@
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="47" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -2159,7 +2221,7 @@
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="47" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2173,7 +2235,7 @@
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -2187,7 +2249,7 @@
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="48" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2201,7 +2263,7 @@
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -2215,7 +2277,7 @@
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="48" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -2229,7 +2291,7 @@
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2243,7 +2305,7 @@
       <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="47" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -2257,7 +2319,7 @@
       <c r="A11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="50" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -2271,7 +2333,7 @@
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="47" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -2285,7 +2347,7 @@
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="47" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2299,7 +2361,7 @@
       <c r="A14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="51" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -2313,7 +2375,7 @@
       <c r="A15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="49" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -2327,7 +2389,7 @@
       <c r="A16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="47" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -2341,7 +2403,7 @@
       <c r="A17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="52" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -2355,7 +2417,7 @@
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="48" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2369,7 +2431,7 @@
       <c r="A19" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="52" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -2383,7 +2445,7 @@
       <c r="A20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="51" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -2397,7 +2459,7 @@
       <c r="A21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="49" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -2411,7 +2473,7 @@
       <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="49" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -2425,7 +2487,7 @@
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="48" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -2439,7 +2501,7 @@
       <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="48" t="s">
         <v>49</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -2453,7 +2515,7 @@
       <c r="A25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="49" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -2467,7 +2529,7 @@
       <c r="A26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="53" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -2481,7 +2543,7 @@
       <c r="A27" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="49" t="s">
         <v>55</v>
       </c>
       <c r="C27" s="18" t="s">
@@ -2495,7 +2557,7 @@
       <c r="A28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -2509,7 +2571,7 @@
       <c r="A29" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="54" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -2523,7 +2585,7 @@
       <c r="A30" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="47" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -2537,7 +2599,7 @@
       <c r="A31" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="48" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -2551,7 +2613,7 @@
       <c r="A32" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="48" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -2565,7 +2627,7 @@
       <c r="A33" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="47" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -2579,7 +2641,7 @@
       <c r="A34" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="48" t="s">
         <v>69</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -2593,7 +2655,7 @@
       <c r="A35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="47" t="s">
         <v>71</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -2607,7 +2669,7 @@
       <c r="A36" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -2621,7 +2683,7 @@
       <c r="A37" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="47" t="s">
         <v>75</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -2635,7 +2697,7 @@
       <c r="A38" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="55" t="s">
         <v>77</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -2649,7 +2711,7 @@
       <c r="A39" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="47" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -2663,7 +2725,7 @@
       <c r="A40" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="47" t="s">
         <v>81</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -2677,7 +2739,7 @@
       <c r="A41" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="47" t="s">
         <v>83</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -2691,7 +2753,7 @@
       <c r="A42" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="47" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -2705,7 +2767,7 @@
       <c r="A43" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="53" t="s">
         <v>87</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -2719,7 +2781,7 @@
       <c r="A44" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="48" t="s">
         <v>89</v>
       </c>
       <c r="C44" s="8" t="s">
@@ -2733,7 +2795,7 @@
       <c r="A45" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="54" t="s">
         <v>91</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -2747,7 +2809,7 @@
       <c r="A46" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="49" t="s">
         <v>93</v>
       </c>
       <c r="C46" s="10" t="s">
@@ -2761,7 +2823,7 @@
       <c r="A47" t="s">
         <v>95</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="56" t="s">
         <v>95</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -2775,7 +2837,7 @@
       <c r="A48" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="49" t="s">
         <v>97</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -2789,7 +2851,7 @@
       <c r="A49" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="57" t="s">
         <v>99</v>
       </c>
       <c r="C49" s="21" t="s">
@@ -2803,7 +2865,7 @@
       <c r="A50" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="47" t="s">
         <v>101</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -2817,7 +2879,7 @@
       <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="49" t="s">
         <v>101</v>
       </c>
       <c r="C51" s="6" t="s">
@@ -2831,7 +2893,7 @@
       <c r="A52" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="47" t="s">
         <v>104</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -2845,7 +2907,7 @@
       <c r="A53" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="47" t="s">
         <v>106</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -2859,7 +2921,7 @@
       <c r="A54" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="47" t="s">
         <v>108</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -2873,7 +2935,7 @@
       <c r="A55" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="58" t="s">
         <v>110</v>
       </c>
       <c r="C55" s="6" t="s">
@@ -2887,7 +2949,7 @@
       <c r="A56" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B56" s="54" t="s">
         <v>112</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -2901,7 +2963,7 @@
       <c r="A57" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="47" t="s">
         <v>114</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -2915,7 +2977,7 @@
       <c r="A58" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="48" t="s">
         <v>116</v>
       </c>
       <c r="C58" s="8" t="s">
@@ -2929,7 +2991,7 @@
       <c r="A59" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="47" t="s">
         <v>118</v>
       </c>
       <c r="C59" s="8" t="s">
@@ -2943,7 +3005,7 @@
       <c r="A60" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="48" t="s">
         <v>120</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -2957,7 +3019,7 @@
       <c r="A61" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="47" t="s">
         <v>122</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -2971,7 +3033,7 @@
       <c r="A62" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="52" t="s">
         <v>124</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -2985,7 +3047,7 @@
       <c r="A63" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="47" t="s">
         <v>126</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -2999,7 +3061,7 @@
       <c r="A64" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="47" t="s">
         <v>128</v>
       </c>
       <c r="C64" s="6" t="s">
@@ -3013,7 +3075,7 @@
       <c r="A65" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="47" t="s">
         <v>130</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -3027,7 +3089,7 @@
       <c r="A66" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="47" t="s">
         <v>132</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -3041,7 +3103,7 @@
       <c r="A67" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="53" t="s">
         <v>134</v>
       </c>
       <c r="C67" s="18" t="s">
@@ -3055,7 +3117,7 @@
       <c r="A68" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="54" t="s">
         <v>136</v>
       </c>
       <c r="C68" s="4" t="s">
@@ -3069,7 +3131,7 @@
       <c r="A69" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="47" t="s">
         <v>138</v>
       </c>
       <c r="C69" s="4" t="s">
@@ -3083,7 +3145,7 @@
       <c r="A70" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="48" t="s">
         <v>140</v>
       </c>
       <c r="C70" s="8" t="s">
@@ -3097,7 +3159,7 @@
       <c r="A71" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="47" t="s">
         <v>141</v>
       </c>
       <c r="C71" s="9" t="s">
@@ -3111,7 +3173,7 @@
       <c r="A72" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="47" t="s">
         <v>143</v>
       </c>
       <c r="C72" s="6" t="s">
@@ -3125,7 +3187,7 @@
       <c r="A73" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="51" t="s">
         <v>145</v>
       </c>
       <c r="C73" s="4" t="s">
@@ -3139,7 +3201,7 @@
       <c r="A74" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="47" t="s">
         <v>147</v>
       </c>
       <c r="C74" s="4" t="s">
@@ -3153,7 +3215,7 @@
       <c r="A75" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="47" t="s">
         <v>149</v>
       </c>
       <c r="C75" s="8" t="s">
@@ -3167,7 +3229,7 @@
       <c r="A76" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="49" t="s">
         <v>151</v>
       </c>
       <c r="C76" s="18" t="s">
@@ -3181,7 +3243,7 @@
       <c r="A77" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="B77" s="23" t="s">
+      <c r="B77" s="54" t="s">
         <v>153</v>
       </c>
       <c r="C77" s="8" t="s">
@@ -3195,7 +3257,7 @@
       <c r="A78" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="47" t="s">
         <v>155</v>
       </c>
       <c r="C78" s="24" t="s">
@@ -3209,7 +3271,7 @@
       <c r="A79" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="47" t="s">
         <v>157</v>
       </c>
       <c r="C79" s="24" t="s">
@@ -3223,7 +3285,7 @@
       <c r="A80" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="52" t="s">
         <v>158</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -3237,7 +3299,7 @@
       <c r="A81" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="47" t="s">
         <v>160</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -3251,7 +3313,7 @@
       <c r="A82" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="19" t="s">
+      <c r="B82" s="54" t="s">
         <v>162</v>
       </c>
       <c r="C82" s="4" t="s">
@@ -3265,7 +3327,7 @@
       <c r="A83" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="47" t="s">
         <v>164</v>
       </c>
       <c r="C83" s="8" t="s">
@@ -3279,7 +3341,7 @@
       <c r="A84" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B84" s="48" t="s">
         <v>166</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -3293,7 +3355,7 @@
       <c r="A85" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="47" t="s">
         <v>168</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -3307,7 +3369,7 @@
       <c r="A86" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="47" t="s">
         <v>170</v>
       </c>
       <c r="C86" s="4" t="s">
@@ -3321,7 +3383,7 @@
       <c r="A87" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="47" t="s">
         <v>172</v>
       </c>
       <c r="C87" s="9" t="s">
@@ -3335,7 +3397,7 @@
       <c r="A88" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="47" t="s">
         <v>174</v>
       </c>
       <c r="C88" s="4" t="s">
@@ -3349,7 +3411,7 @@
       <c r="A89" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="25" t="s">
+      <c r="B89" s="53" t="s">
         <v>176</v>
       </c>
       <c r="C89" s="11" t="s">
@@ -3363,7 +3425,7 @@
       <c r="A90" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="49" t="s">
         <v>178</v>
       </c>
       <c r="C90" s="6" t="s">
@@ -3377,7 +3439,7 @@
       <c r="A91" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="47" t="s">
         <v>180</v>
       </c>
       <c r="C91" s="8" t="s">
@@ -3391,7 +3453,7 @@
       <c r="A92" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="47" t="s">
         <v>182</v>
       </c>
       <c r="C92" s="8" t="s">
@@ -3405,7 +3467,7 @@
       <c r="A93" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="47" t="s">
         <v>184</v>
       </c>
       <c r="C93" s="4" t="s">
@@ -3419,7 +3481,7 @@
       <c r="A94" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B94" s="48" t="s">
         <v>186</v>
       </c>
       <c r="C94" s="8" t="s">
@@ -3433,7 +3495,7 @@
       <c r="A95" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="47" t="s">
         <v>188</v>
       </c>
       <c r="C95" s="8" t="s">
@@ -3447,7 +3509,7 @@
       <c r="A96" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="51" t="s">
         <v>190</v>
       </c>
       <c r="C96" s="4" t="s">
@@ -3461,7 +3523,7 @@
       <c r="A97" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="47" t="s">
         <v>192</v>
       </c>
       <c r="C97" s="4" t="s">
@@ -3475,7 +3537,7 @@
       <c r="A98" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="11" t="s">
+      <c r="B98" s="47" t="s">
         <v>194</v>
       </c>
       <c r="C98" s="8" t="s">
@@ -3489,7 +3551,7 @@
       <c r="A99" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="B99" s="17" t="s">
+      <c r="B99" s="53" t="s">
         <v>196</v>
       </c>
       <c r="C99" s="18" t="s">
@@ -3503,7 +3565,7 @@
       <c r="A100" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="48" t="s">
         <v>198</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -3517,7 +3579,7 @@
       <c r="A101" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B101" s="48" t="s">
         <v>200</v>
       </c>
       <c r="C101" s="4" t="s">
@@ -3531,7 +3593,7 @@
       <c r="A102" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="47" t="s">
         <v>202</v>
       </c>
       <c r="C102" s="8" t="s">
@@ -3545,7 +3607,7 @@
       <c r="A103" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="47" t="s">
         <v>204</v>
       </c>
       <c r="C103" s="4" t="s">
@@ -3559,7 +3621,7 @@
       <c r="A104" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B104" s="49" t="s">
         <v>206</v>
       </c>
       <c r="C104" s="6" t="s">
@@ -3573,7 +3635,7 @@
       <c r="A105" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B105" s="48" t="s">
         <v>208</v>
       </c>
       <c r="C105" s="8" t="s">
@@ -3587,7 +3649,7 @@
       <c r="A106" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B106" s="48" t="s">
         <v>210</v>
       </c>
       <c r="C106" s="8" t="s">
@@ -3601,7 +3663,7 @@
       <c r="A107" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="47" t="s">
         <v>212</v>
       </c>
       <c r="C107" s="4" t="s">
@@ -3615,7 +3677,7 @@
       <c r="A108" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="47" t="s">
         <v>214</v>
       </c>
       <c r="C108" s="4" t="s">
@@ -3629,7 +3691,7 @@
       <c r="A109" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="49" t="s">
         <v>216</v>
       </c>
       <c r="C109" s="6" t="s">
@@ -3643,7 +3705,7 @@
       <c r="A110" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B110" s="6" t="s">
+      <c r="B110" s="49" t="s">
         <v>218</v>
       </c>
       <c r="C110" s="6" t="s">
@@ -3657,7 +3719,7 @@
       <c r="A111" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B111" s="11" t="s">
+      <c r="B111" s="47" t="s">
         <v>220</v>
       </c>
       <c r="C111" s="8" t="s">
@@ -3671,7 +3733,7 @@
       <c r="A112" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="47" t="s">
         <v>222</v>
       </c>
       <c r="C112" s="4" t="s">
@@ -3685,7 +3747,7 @@
       <c r="A113" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B113" s="47" t="s">
         <v>223</v>
       </c>
       <c r="C113" s="4" t="s">
@@ -3699,7 +3761,7 @@
       <c r="A114" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="47" t="s">
         <v>225</v>
       </c>
       <c r="C114" s="8" t="s">
@@ -3713,7 +3775,7 @@
       <c r="A115" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B115" s="11" t="s">
+      <c r="B115" s="47" t="s">
         <v>227</v>
       </c>
       <c r="C115" s="8" t="s">
@@ -3727,7 +3789,7 @@
       <c r="A116" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B116" s="26" t="s">
+      <c r="B116" s="47" t="s">
         <v>229</v>
       </c>
       <c r="C116" s="27" t="s">
@@ -3741,7 +3803,7 @@
       <c r="A117" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B117" s="48" t="s">
         <v>231</v>
       </c>
       <c r="C117" s="4" t="s">
@@ -3755,7 +3817,7 @@
       <c r="A118" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="B118" s="47" t="s">
         <v>233</v>
       </c>
       <c r="C118" s="4" t="s">
@@ -3769,7 +3831,7 @@
       <c r="A119" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B119" s="48" t="s">
         <v>235</v>
       </c>
       <c r="C119" s="4" t="s">
@@ -3783,7 +3845,7 @@
       <c r="A120" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="B120" s="28" t="s">
+      <c r="B120" s="59" t="s">
         <v>237</v>
       </c>
       <c r="C120" s="6" t="s">
@@ -3797,7 +3859,7 @@
       <c r="A121" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="47" t="s">
         <v>239</v>
       </c>
       <c r="C121" s="8" t="s">
@@ -3811,7 +3873,7 @@
       <c r="A122" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="47" t="s">
         <v>241</v>
       </c>
       <c r="C122" s="4" t="s">
@@ -3825,7 +3887,7 @@
       <c r="A123" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="B123" s="16" t="s">
+      <c r="B123" s="52" t="s">
         <v>243</v>
       </c>
       <c r="C123" s="8" t="s">
@@ -3839,7 +3901,7 @@
       <c r="A124" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="47" t="s">
         <v>245</v>
       </c>
       <c r="C124" s="9" t="s">
@@ -3853,7 +3915,7 @@
       <c r="A125" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="47" t="s">
         <v>247</v>
       </c>
       <c r="C125" s="4" t="s">
@@ -3867,7 +3929,7 @@
       <c r="A126" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B126" s="11" t="s">
+      <c r="B126" s="47" t="s">
         <v>249</v>
       </c>
       <c r="C126" s="8" t="s">
@@ -3881,7 +3943,7 @@
       <c r="A127" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B127" s="47" t="s">
         <v>251</v>
       </c>
       <c r="C127" s="9" t="s">
@@ -3895,7 +3957,7 @@
       <c r="A128" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="B128" s="11" t="s">
+      <c r="B128" s="47" t="s">
         <v>253</v>
       </c>
       <c r="C128" s="7" t="s">
@@ -3909,7 +3971,7 @@
       <c r="A129" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="B129" s="19" t="s">
+      <c r="B129" s="54" t="s">
         <v>255</v>
       </c>
       <c r="C129" s="9" t="s">
@@ -3923,7 +3985,7 @@
       <c r="A130" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="47" t="s">
         <v>257</v>
       </c>
       <c r="C130" s="24" t="s">
@@ -3937,7 +3999,7 @@
       <c r="A131" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="47" t="s">
         <v>258</v>
       </c>
       <c r="C131" s="24" t="s">
@@ -3951,7 +4013,7 @@
       <c r="A132" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B132" s="47" t="s">
         <v>259</v>
       </c>
       <c r="C132" s="24" t="s">
@@ -3965,7 +4027,7 @@
       <c r="A133" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="B133" s="9" t="s">
+      <c r="B133" s="48" t="s">
         <v>260</v>
       </c>
       <c r="C133" s="4" t="s">
@@ -3979,7 +4041,7 @@
       <c r="A134" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B134" s="9" t="s">
+      <c r="B134" s="48" t="s">
         <v>262</v>
       </c>
       <c r="C134" s="4" t="s">
@@ -3993,7 +4055,7 @@
       <c r="A135" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="B135" s="11" t="s">
+      <c r="B135" s="47" t="s">
         <v>264</v>
       </c>
       <c r="C135" s="8" t="s">
@@ -4007,7 +4069,7 @@
       <c r="A136" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="B136" s="29" t="s">
+      <c r="B136" s="60" t="s">
         <v>266</v>
       </c>
       <c r="C136" s="30" t="s">
@@ -4021,7 +4083,7 @@
       <c r="A137" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B137" s="6" t="s">
+      <c r="B137" s="49" t="s">
         <v>268</v>
       </c>
       <c r="C137" s="6" t="s">
@@ -4035,7 +4097,7 @@
       <c r="A138" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B138" s="5" t="s">
+      <c r="B138" s="47" t="s">
         <v>270</v>
       </c>
       <c r="C138" s="4" t="s">
@@ -4049,7 +4111,7 @@
       <c r="A139" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="B139" s="31" t="s">
+      <c r="B139" s="58" t="s">
         <v>272</v>
       </c>
       <c r="C139" s="8" t="s">
@@ -4063,7 +4125,7 @@
       <c r="A140" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B140" s="49" t="s">
         <v>274</v>
       </c>
       <c r="C140" s="6" t="s">
@@ -4077,7 +4139,7 @@
       <c r="A141" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="B141" s="32" t="s">
+      <c r="B141" s="60" t="s">
         <v>276</v>
       </c>
       <c r="C141" s="8" t="s">
@@ -4091,7 +4153,7 @@
       <c r="A142" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="B142" s="23" t="s">
+      <c r="B142" s="54" t="s">
         <v>278</v>
       </c>
       <c r="C142" s="8" t="s">
@@ -4105,7 +4167,7 @@
       <c r="A143" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B143" s="6" t="s">
+      <c r="B143" s="49" t="s">
         <v>280</v>
       </c>
       <c r="C143" s="6" t="s">
@@ -4119,7 +4181,7 @@
       <c r="A144" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="B144" s="10" t="s">
+      <c r="B144" s="49" t="s">
         <v>282</v>
       </c>
       <c r="C144" s="10" t="s">
@@ -4133,7 +4195,7 @@
       <c r="A145" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B145" s="47" t="s">
         <v>284</v>
       </c>
       <c r="C145" s="4" t="s">
@@ -4147,7 +4209,7 @@
       <c r="A146" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="B146" s="16" t="s">
+      <c r="B146" s="52" t="s">
         <v>286</v>
       </c>
       <c r="C146" s="8" t="s">
@@ -4161,7 +4223,7 @@
       <c r="A147" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B147" s="5" t="s">
+      <c r="B147" s="47" t="s">
         <v>288</v>
       </c>
       <c r="C147" s="4" t="s">
@@ -4175,7 +4237,7 @@
       <c r="A148" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B148" s="9" t="s">
+      <c r="B148" s="48" t="s">
         <v>290</v>
       </c>
       <c r="C148" s="4" t="s">
@@ -4189,7 +4251,7 @@
       <c r="A149" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="B149" s="13" t="s">
+      <c r="B149" s="57" t="s">
         <v>292</v>
       </c>
       <c r="C149" s="13" t="s">
@@ -4203,7 +4265,7 @@
       <c r="A150" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="47" t="s">
         <v>293</v>
       </c>
       <c r="C150" s="8" t="s">
@@ -4217,7 +4279,7 @@
       <c r="A151" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B151" s="5" t="s">
+      <c r="B151" s="47" t="s">
         <v>295</v>
       </c>
       <c r="C151" s="4" t="s">
@@ -4231,7 +4293,7 @@
       <c r="A152" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B152" s="6" t="s">
+      <c r="B152" s="49" t="s">
         <v>297</v>
       </c>
       <c r="C152" s="6" t="s">
@@ -4245,7 +4307,7 @@
       <c r="A153" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="B153" s="11" t="s">
+      <c r="B153" s="47" t="s">
         <v>299</v>
       </c>
       <c r="C153" s="8" t="s">
@@ -4259,7 +4321,7 @@
       <c r="A154" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="47" t="s">
         <v>301</v>
       </c>
       <c r="C154" s="4" t="s">
@@ -4273,7 +4335,7 @@
       <c r="A155" s="32" t="s">
         <v>303</v>
       </c>
-      <c r="B155" s="32" t="s">
+      <c r="B155" s="60" t="s">
         <v>303</v>
       </c>
       <c r="C155" s="33" t="s">
@@ -4287,7 +4349,7 @@
       <c r="A156" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="B156" s="11" t="s">
+      <c r="B156" s="47" t="s">
         <v>305</v>
       </c>
       <c r="C156" s="8" t="s">
@@ -4301,7 +4363,7 @@
       <c r="A157" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="B157" s="6" t="s">
+      <c r="B157" s="49" t="s">
         <v>307</v>
       </c>
       <c r="C157" s="6" t="s">
@@ -4315,7 +4377,7 @@
       <c r="A158" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="B158" s="7" t="s">
+      <c r="B158" s="48" t="s">
         <v>309</v>
       </c>
       <c r="C158" s="8" t="s">
@@ -4329,7 +4391,7 @@
       <c r="A159" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="B159" s="19" t="s">
+      <c r="B159" s="54" t="s">
         <v>311</v>
       </c>
       <c r="C159" s="4" t="s">
@@ -4343,7 +4405,7 @@
       <c r="A160" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B160" s="47" t="s">
         <v>312</v>
       </c>
       <c r="C160" s="4" t="s">
@@ -4357,7 +4419,7 @@
       <c r="A161" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="B161" s="16" t="s">
+      <c r="B161" s="52" t="s">
         <v>314</v>
       </c>
       <c r="C161" s="8" t="s">
@@ -4371,7 +4433,7 @@
       <c r="A162" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="B162" s="11" t="s">
+      <c r="B162" s="47" t="s">
         <v>316</v>
       </c>
       <c r="C162" s="8" t="s">
@@ -4385,7 +4447,7 @@
       <c r="A163" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="B163" s="11" t="s">
+      <c r="B163" s="47" t="s">
         <v>318</v>
       </c>
       <c r="C163" s="8" t="s">
@@ -4399,7 +4461,7 @@
       <c r="A164" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B164" s="47" t="s">
         <v>320</v>
       </c>
       <c r="C164" s="5" t="s">
@@ -4413,7 +4475,7 @@
       <c r="A165" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="B165" s="47" t="s">
         <v>321</v>
       </c>
       <c r="C165" s="24" t="s">
@@ -4427,7 +4489,7 @@
       <c r="A166" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="B166" s="6" t="s">
+      <c r="B166" s="49" t="s">
         <v>323</v>
       </c>
       <c r="C166" s="18" t="s">
@@ -4441,7 +4503,7 @@
       <c r="A167" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="B167" s="18" t="s">
+      <c r="B167" s="57" t="s">
         <v>325</v>
       </c>
       <c r="C167" s="34" t="s">
@@ -4455,7 +4517,7 @@
       <c r="A168" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B168" s="6" t="s">
+      <c r="B168" s="49" t="s">
         <v>327</v>
       </c>
       <c r="C168" s="18" t="s">
@@ -4469,7 +4531,7 @@
       <c r="A169" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="B169" s="6" t="s">
+      <c r="B169" s="49" t="s">
         <v>329</v>
       </c>
       <c r="C169" s="6" t="s">
@@ -4483,7 +4545,7 @@
       <c r="A170" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B170" s="18" t="s">
+      <c r="B170" s="57" t="s">
         <v>331</v>
       </c>
       <c r="C170" s="4" t="s">
@@ -4497,7 +4559,7 @@
       <c r="A171" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="B171" s="35" t="s">
+      <c r="B171" s="50" t="s">
         <v>333</v>
       </c>
       <c r="C171" s="34" t="s">
@@ -4511,7 +4573,7 @@
       <c r="A172" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B172" s="47" t="s">
         <v>335</v>
       </c>
       <c r="C172" s="9" t="s">
@@ -4525,7 +4587,7 @@
       <c r="A173" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="B173" s="47" t="s">
         <v>337</v>
       </c>
       <c r="C173" s="6" t="s">
@@ -4539,7 +4601,7 @@
       <c r="A174" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B174" s="18" t="s">
+      <c r="B174" s="57" t="s">
         <v>339</v>
       </c>
       <c r="C174" s="4" t="s">
@@ -4553,7 +4615,7 @@
       <c r="A175" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="B175" s="22" t="s">
+      <c r="B175" s="58" t="s">
         <v>341</v>
       </c>
       <c r="C175" s="6" t="s">
@@ -4567,7 +4629,7 @@
       <c r="A176" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="B176" s="6" t="s">
+      <c r="B176" s="49" t="s">
         <v>343</v>
       </c>
       <c r="C176" s="6" t="s">
@@ -4581,7 +4643,7 @@
       <c r="A177" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="B177" s="18" t="s">
+      <c r="B177" s="57" t="s">
         <v>345</v>
       </c>
       <c r="C177" s="4" t="s">
@@ -4595,7 +4657,7 @@
       <c r="A178" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B178" s="5" t="s">
+      <c r="B178" s="47" t="s">
         <v>347</v>
       </c>
       <c r="C178" s="4" t="s">
@@ -4609,7 +4671,7 @@
       <c r="A179" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="B179" s="18" t="s">
+      <c r="B179" s="57" t="s">
         <v>349</v>
       </c>
       <c r="C179" s="4" t="s">
@@ -4623,7 +4685,7 @@
       <c r="A180" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="B180" s="18" t="s">
+      <c r="B180" s="57" t="s">
         <v>351</v>
       </c>
       <c r="C180" s="34" t="s">
@@ -4637,7 +4699,7 @@
       <c r="A181" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="B181" s="9" t="s">
+      <c r="B181" s="48" t="s">
         <v>353</v>
       </c>
       <c r="C181" s="4" t="s">
@@ -4651,7 +4713,7 @@
       <c r="A182" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="B182" s="18" t="s">
+      <c r="B182" s="13" t="s">
         <v>479</v>
       </c>
       <c r="C182" s="4" t="s">
@@ -4665,7 +4727,7 @@
       <c r="A183" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="B183" s="17" t="s">
+      <c r="B183" s="53" t="s">
         <v>357</v>
       </c>
       <c r="C183" s="6" t="s">
@@ -4679,7 +4741,7 @@
       <c r="A184" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="B184" s="22" t="s">
+      <c r="B184" s="58" t="s">
         <v>359</v>
       </c>
       <c r="C184" s="4" t="s">
@@ -4693,7 +4755,7 @@
       <c r="A185" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="B185" s="18" t="s">
+      <c r="B185" s="57" t="s">
         <v>361</v>
       </c>
       <c r="C185" s="4" t="s">
@@ -4707,7 +4769,7 @@
       <c r="A186" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="B186" s="6" t="s">
+      <c r="B186" s="49" t="s">
         <v>363</v>
       </c>
       <c r="C186" s="34" t="s">
@@ -4721,7 +4783,7 @@
       <c r="A187" s="36" t="s">
         <v>365</v>
       </c>
-      <c r="B187" s="36" t="s">
+      <c r="B187" s="61" t="s">
         <v>365</v>
       </c>
       <c r="C187" s="4" t="s">
@@ -4735,7 +4797,7 @@
       <c r="A188" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="B188" s="18" t="s">
+      <c r="B188" s="57" t="s">
         <v>367</v>
       </c>
       <c r="C188" s="4" t="s">
@@ -4749,7 +4811,7 @@
       <c r="A189" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="B189" s="17" t="s">
+      <c r="B189" s="53" t="s">
         <v>369</v>
       </c>
       <c r="C189" s="6" t="s">
@@ -4763,7 +4825,7 @@
       <c r="A190" s="18" t="s">
         <v>371</v>
       </c>
-      <c r="B190" s="18" t="s">
+      <c r="B190" s="57" t="s">
         <v>371</v>
       </c>
       <c r="C190" s="18" t="s">
@@ -4777,7 +4839,7 @@
       <c r="A191" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="B191" s="18" t="s">
+      <c r="B191" s="57" t="s">
         <v>373</v>
       </c>
       <c r="C191" s="4" t="s">
@@ -4791,7 +4853,7 @@
       <c r="A192" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="B192" s="5" t="s">
+      <c r="B192" s="47" t="s">
         <v>375</v>
       </c>
       <c r="C192" s="5" t="s">
@@ -4805,7 +4867,7 @@
       <c r="A193" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="B193" s="5" t="s">
+      <c r="B193" s="47" t="s">
         <v>376</v>
       </c>
       <c r="C193" s="4" t="s">
@@ -4819,7 +4881,7 @@
       <c r="A194" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="B194" s="18" t="s">
+      <c r="B194" s="57" t="s">
         <v>378</v>
       </c>
       <c r="C194" s="4" t="s">
@@ -4833,7 +4895,7 @@
       <c r="A195" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="B195" s="18" t="s">
+      <c r="B195" s="57" t="s">
         <v>380</v>
       </c>
       <c r="C195" s="4" t="s">
@@ -4847,7 +4909,7 @@
       <c r="A196" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="B196" s="18" t="s">
+      <c r="B196" s="57" t="s">
         <v>382</v>
       </c>
       <c r="C196" s="4" t="s">
@@ -4861,7 +4923,7 @@
       <c r="A197" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="B197" s="17" t="s">
+      <c r="B197" s="53" t="s">
         <v>384</v>
       </c>
       <c r="C197" s="6" t="s">
@@ -4875,7 +4937,7 @@
       <c r="A198" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="B198" s="18" t="s">
+      <c r="B198" s="57" t="s">
         <v>386</v>
       </c>
       <c r="C198" s="4" t="s">
@@ -4889,7 +4951,7 @@
       <c r="A199" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="B199" s="18" t="s">
+      <c r="B199" s="57" t="s">
         <v>388</v>
       </c>
       <c r="C199" s="4" t="s">
@@ -4903,7 +4965,7 @@
       <c r="A200" s="35" t="s">
         <v>390</v>
       </c>
-      <c r="B200" s="35" t="s">
+      <c r="B200" s="50" t="s">
         <v>390</v>
       </c>
       <c r="C200" s="9" t="s">
@@ -4917,7 +4979,7 @@
       <c r="A201" s="22" t="s">
         <v>392</v>
       </c>
-      <c r="B201" s="22" t="s">
+      <c r="B201" s="58" t="s">
         <v>392</v>
       </c>
       <c r="C201" s="22" t="s">
@@ -4931,7 +4993,7 @@
       <c r="A202" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="B202" s="17" t="s">
+      <c r="B202" s="53" t="s">
         <v>394</v>
       </c>
       <c r="C202" s="6" t="s">
@@ -4945,7 +5007,7 @@
       <c r="A203" s="35" t="s">
         <v>396</v>
       </c>
-      <c r="B203" s="35" t="s">
+      <c r="B203" s="50" t="s">
         <v>396</v>
       </c>
       <c r="C203" s="9" t="s">
@@ -4959,7 +5021,7 @@
       <c r="A204" s="18" t="s">
         <v>398</v>
       </c>
-      <c r="B204" s="18" t="s">
+      <c r="B204" s="57" t="s">
         <v>398</v>
       </c>
       <c r="C204" s="9" t="s">
@@ -4973,7 +5035,7 @@
       <c r="A205" s="18" t="s">
         <v>400</v>
       </c>
-      <c r="B205" s="18" t="s">
+      <c r="B205" s="57" t="s">
         <v>400</v>
       </c>
       <c r="C205" s="9" t="s">
@@ -4987,7 +5049,7 @@
       <c r="A206" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="B206" s="9" t="s">
+      <c r="B206" s="48" t="s">
         <v>402</v>
       </c>
       <c r="C206" s="9" t="s">
@@ -5001,7 +5063,7 @@
       <c r="A207" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="B207" s="18" t="s">
+      <c r="B207" s="57" t="s">
         <v>404</v>
       </c>
       <c r="C207" s="9" t="s">
@@ -5015,7 +5077,7 @@
       <c r="A208" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="B208" s="5" t="s">
+      <c r="B208" s="47" t="s">
         <v>406</v>
       </c>
       <c r="C208" s="5" t="s">
@@ -5029,7 +5091,7 @@
       <c r="A209" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="B209" s="5" t="s">
+      <c r="B209" s="47" t="s">
         <v>407</v>
       </c>
       <c r="C209" s="6" t="s">
@@ -5043,7 +5105,7 @@
       <c r="A210" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="B210" s="11" t="s">
+      <c r="B210" s="47" t="s">
         <v>409</v>
       </c>
       <c r="C210" s="8" t="s">
@@ -5057,7 +5119,7 @@
       <c r="A211" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="B211" s="11" t="s">
+      <c r="B211" s="47" t="s">
         <v>411</v>
       </c>
       <c r="C211" s="8" t="s">
@@ -5071,7 +5133,7 @@
       <c r="A212" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="B212" s="7" t="s">
+      <c r="B212" s="48" t="s">
         <v>413</v>
       </c>
       <c r="C212" s="8" t="s">
@@ -5085,7 +5147,7 @@
       <c r="A213" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="B213" s="6" t="s">
+      <c r="B213" s="49" t="s">
         <v>415</v>
       </c>
       <c r="C213" s="6" t="s">
@@ -5099,7 +5161,7 @@
       <c r="A214" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="B214" s="6" t="s">
+      <c r="B214" s="49" t="s">
         <v>417</v>
       </c>
       <c r="C214" s="6" t="s">
@@ -5113,7 +5175,7 @@
       <c r="A215" s="7" t="s">
         <v>418</v>
       </c>
-      <c r="B215" s="7" t="s">
+      <c r="B215" s="48" t="s">
         <v>418</v>
       </c>
       <c r="C215" s="8" t="s">
@@ -5127,7 +5189,7 @@
       <c r="A216" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="B216" s="5" t="s">
+      <c r="B216" s="47" t="s">
         <v>420</v>
       </c>
       <c r="C216" s="4" t="s">
@@ -5141,7 +5203,7 @@
       <c r="A217" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="B217" s="7" t="s">
+      <c r="B217" s="48" t="s">
         <v>422</v>
       </c>
       <c r="C217" s="7" t="s">
@@ -5155,7 +5217,7 @@
       <c r="A218" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="B218" s="5" t="s">
+      <c r="B218" s="47" t="s">
         <v>424</v>
       </c>
       <c r="C218" s="9" t="s">
@@ -5169,7 +5231,7 @@
       <c r="A219" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="B219" s="11" t="s">
+      <c r="B219" s="47" t="s">
         <v>426</v>
       </c>
       <c r="C219" s="32" t="s">
@@ -5183,7 +5245,7 @@
       <c r="A220" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="B220" s="5" t="s">
+      <c r="B220" s="47" t="s">
         <v>428</v>
       </c>
       <c r="C220" s="9" t="s">
@@ -5197,7 +5259,7 @@
       <c r="A221" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="B221" s="11" t="s">
+      <c r="B221" s="47" t="s">
         <v>430</v>
       </c>
       <c r="C221" s="7" t="s">
@@ -5211,7 +5273,7 @@
       <c r="A222" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="B222" s="9" t="s">
+      <c r="B222" s="48" t="s">
         <v>431</v>
       </c>
       <c r="C222" s="9" t="s">
@@ -5225,7 +5287,7 @@
       <c r="A223" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="B223" s="11" t="s">
+      <c r="B223" s="47" t="s">
         <v>433</v>
       </c>
       <c r="C223" s="7" t="s">
@@ -5239,7 +5301,7 @@
       <c r="A224" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="B224" s="19" t="s">
+      <c r="B224" s="54" t="s">
         <v>435</v>
       </c>
       <c r="C224" s="9" t="s">
@@ -5253,7 +5315,7 @@
       <c r="A225" s="11" t="s">
         <v>437</v>
       </c>
-      <c r="B225" s="11" t="s">
+      <c r="B225" s="47" t="s">
         <v>437</v>
       </c>
       <c r="C225" s="8" t="s">
@@ -5267,7 +5329,7 @@
       <c r="A226" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="B226" s="14" t="s">
+      <c r="B226" s="51" t="s">
         <v>439</v>
       </c>
       <c r="C226" s="9" t="s">
@@ -5281,7 +5343,7 @@
       <c r="A227" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="B227" s="6" t="s">
+      <c r="B227" s="49" t="s">
         <v>441</v>
       </c>
       <c r="C227" s="6" t="s">
@@ -5295,7 +5357,7 @@
       <c r="A228" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="B228" s="11" t="s">
+      <c r="B228" s="47" t="s">
         <v>443</v>
       </c>
       <c r="C228" s="7" t="s">
@@ -5309,7 +5371,7 @@
       <c r="A229" s="6" t="s">
         <v>445</v>
       </c>
-      <c r="B229" s="6" t="s">
+      <c r="B229" s="49" t="s">
         <v>445</v>
       </c>
       <c r="C229" s="6" t="s">
@@ -5323,7 +5385,7 @@
       <c r="A230" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="B230" s="11" t="s">
+      <c r="B230" s="47" t="s">
         <v>447</v>
       </c>
       <c r="C230" s="8" t="s">
@@ -5337,7 +5399,7 @@
       <c r="A231" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="B231" s="5" t="s">
+      <c r="B231" s="47" t="s">
         <v>449</v>
       </c>
       <c r="C231" s="6" t="s">
@@ -5351,7 +5413,7 @@
       <c r="A232" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="B232" s="18" t="s">
+      <c r="B232" s="57" t="s">
         <v>450</v>
       </c>
       <c r="C232" s="9" t="s">
@@ -5365,7 +5427,7 @@
       <c r="A233" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="B233" s="5" t="s">
+      <c r="B233" s="47" t="s">
         <v>452</v>
       </c>
       <c r="C233" s="9" t="s">
@@ -5379,7 +5441,7 @@
       <c r="A234" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="B234" s="5" t="s">
+      <c r="B234" s="47" t="s">
         <v>454</v>
       </c>
       <c r="C234" s="9" t="s">
@@ -5393,7 +5455,7 @@
       <c r="A235" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="B235" s="11" t="s">
+      <c r="B235" s="47" t="s">
         <v>456</v>
       </c>
       <c r="C235" s="7" t="s">
@@ -5407,7 +5469,7 @@
       <c r="A236" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="B236" s="11" t="s">
+      <c r="B236" s="47" t="s">
         <v>458</v>
       </c>
       <c r="C236" s="7" t="s">
@@ -5421,7 +5483,7 @@
       <c r="A237" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="B237" s="11" t="s">
+      <c r="B237" s="47" t="s">
         <v>460</v>
       </c>
       <c r="C237" s="8" t="s">
@@ -5435,7 +5497,7 @@
       <c r="A238" s="9" t="s">
         <v>462</v>
       </c>
-      <c r="B238" s="9" t="s">
+      <c r="B238" s="48" t="s">
         <v>462</v>
       </c>
       <c r="C238" s="9" t="s">
@@ -5449,7 +5511,7 @@
       <c r="A239" s="37" t="s">
         <v>464</v>
       </c>
-      <c r="B239" s="37" t="s">
+      <c r="B239" s="48" t="s">
         <v>464</v>
       </c>
       <c r="C239" s="37" t="s">
@@ -5463,7 +5525,7 @@
       <c r="A240" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="B240" s="9" t="s">
+      <c r="B240" s="48" t="s">
         <v>466</v>
       </c>
       <c r="C240" s="9" t="s">
@@ -5477,7 +5539,7 @@
       <c r="A241" s="38" t="s">
         <v>468</v>
       </c>
-      <c r="B241" s="38" t="s">
+      <c r="B241" s="62" t="s">
         <v>468</v>
       </c>
       <c r="C241" s="38" t="s">
@@ -5491,7 +5553,7 @@
       <c r="A242" s="38" t="s">
         <v>470</v>
       </c>
-      <c r="B242" s="38" t="s">
+      <c r="B242" s="62" t="s">
         <v>470</v>
       </c>
       <c r="C242" s="38" t="s">
@@ -5505,7 +5567,7 @@
       <c r="A243" s="38" t="s">
         <v>472</v>
       </c>
-      <c r="B243" s="38" t="s">
+      <c r="B243" s="62" t="s">
         <v>472</v>
       </c>
       <c r="C243" s="38" t="s">
@@ -5519,7 +5581,7 @@
       <c r="A244" s="39" t="s">
         <v>474</v>
       </c>
-      <c r="B244" s="39" t="s">
+      <c r="B244" s="63" t="s">
         <v>474</v>
       </c>
       <c r="C244" s="40" t="s">
@@ -5533,7 +5595,7 @@
       <c r="A245" s="41" t="s">
         <v>476</v>
       </c>
-      <c r="B245" s="41" t="s">
+      <c r="B245" s="63" t="s">
         <v>476</v>
       </c>
       <c r="C245" s="42" t="s">
@@ -5545,7 +5607,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="40"/>
-      <c r="B246" s="40"/>
+      <c r="B246" s="64"/>
       <c r="C246" s="40"/>
       <c r="D246" s="44"/>
     </row>

</xml_diff>